<commit_message>
added gdd and tasks planner
</commit_message>
<xml_diff>
--- a/MixorcerersTODO.xlsx
+++ b/MixorcerersTODO.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Pitch" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -41,6 +42,90 @@
   </si>
   <si>
     <t xml:space="preserve">Write Local Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Working title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixorcerers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixorcerers is a turn based 1v1 game that combines rts elements with the unlimited power of a mage. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genre(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target audience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Universal ESRB – suitable 13 and up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Selling Points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Power Fantasy, Interesting Combat System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Experience and Game POV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player is a mage. Setting is cheerful medieaval. Archmage fantasy. Power, scheming, accomplishment, gumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual and Audio Style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reminiscent of FE7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game World Fiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1v1 arena, maybe some mcguffin, some kinda astral projection to keep the constant battles canon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monetization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feed me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platform(s), Technology, and Scope (brief)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC and mobile. Godot. Maybe a couple more months, team of me. Couple more months? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Loops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1v1 laddering is a classic loop of self improvement. The rich variety of strategies will also cause people to come back again. The different types of maps and some kind of randomness in gaining orbs will stop the meta from getting stale. Currently im thinking of bases to capture as well as worker harassment for magycke. I expect to see a dedicated but small community that will play the game for many years, and hopefully I can hand off balance and such to them eventually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objectives and Progression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theres a tutorial, and then the ladder. There will be a leaderboard.While battling people may find stuff that improves their lobby screen which is like their personal den.In the future I may add puzzles if Im jobless. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplayer Server,Replays, Client – Game, Menus, DisplayShowcase , Main webserver that does leaderboard, display showcase,matchmaking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The interactivity is nice keyboard shortcuts for everything. The player moves the cursor which interacts with the units and structures, then uses the menu to execute commands. The combat works by casting spells on the map</t>
   </si>
 </sst>
 </file>
@@ -55,6 +140,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -72,7 +158,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +181,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF6D"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFF7D1D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D1D5"/>
+        <bgColor rgb="FFDDE8CB"/>
       </patternFill>
     </fill>
   </fills>
@@ -132,25 +236,45 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,12 +322,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFDDE8CB"/>
+      <rgbColor rgb="FFFFFF6D"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -338,14 +462,14 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.99"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,12 +490,9 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -380,7 +501,7 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -393,4 +514,144 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="49.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more UI wireframe for the local server
</commit_message>
<xml_diff>
--- a/MixorcerersTODO.xlsx
+++ b/MixorcerersTODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t xml:space="preserve">Write Local Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client wireframe to test server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Local Server Scene</t>
   </si>
   <si>
     <t xml:space="preserve">Working title</t>
@@ -158,7 +164,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +187,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
@@ -236,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,23 +269,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,7 +346,7 @@
       <rgbColor rgb="FFF7D1D5"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -460,10 +476,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,6 +519,16 @@
       </c>
       <c r="C4" s="1" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -523,126 +549,126 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="115.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>18</v>
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>20</v>
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>22</v>
+      <c r="A9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
+      <c r="A10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>26</v>
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="49.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>28</v>
+      <c r="A13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>30</v>
+      <c r="A14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>32</v>
+      <c r="A15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>34</v>
+      <c r="A16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally finished the skeleton of the game. Perfect for gorgeous looks, merge ASAP
</commit_message>
<xml_diff>
--- a/MixorcerersTODO.xlsx
+++ b/MixorcerersTODO.xlsx
@@ -47,9 +47,6 @@
     <t xml:space="preserve">Client wireframe to test server</t>
   </si>
   <si>
-    <t xml:space="preserve">Create Local Server Scene</t>
-  </si>
-  <si>
     <t xml:space="preserve">Settings Page</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">Server set udp destination(should be same as client udp listener)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low  processor mode in menus</t>
   </si>
   <si>
     <t xml:space="preserve">Working title</t>
@@ -176,7 +176,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +205,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -260,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -289,19 +295,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -488,10 +498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,7 +536,7 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -539,27 +549,33 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B6" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -591,114 +607,114 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="49.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>